<commit_message>
intermediate revision - refactored the code, temporarily commented the Excel 2007 due to observed IllegalStateException
</commit_message>
<xml_diff>
--- a/src/test/resources/data_2007.xlsx
+++ b/src/test/resources/data_2007.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">spock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">there is no such thing</t>
   </si>
 </sst>
 </file>
@@ -141,15 +138,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -196,21 +193,198 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
intermediate revision - fixed row/ column iteraror error triggered exception when loading test data from Excel 2007
</commit_message>
<xml_diff>
--- a/src/test/resources/data_2007.xlsx
+++ b/src/test/resources/data_2007.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">spock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">there is no such thing</t>
   </si>
 </sst>
 </file>
@@ -141,17 +138,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.73"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -198,17 +193,194 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>